<commit_message>
done with the algorithm
</commit_message>
<xml_diff>
--- a/Timetable Project.xlsx
+++ b/Timetable Project.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/riley/dev/timetable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCA642E-3AE5-874D-87BD-3203DDA97018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C702FC31-43A8-D04B-A982-E131D028DFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="3100" windowWidth="20920" windowHeight="12980" xr2:uid="{B9BCC66F-D43E-1749-A212-4ECD819803F3}"/>
+    <workbookView xWindow="2160" yWindow="3100" windowWidth="20920" windowHeight="12980" activeTab="3" xr2:uid="{B9BCC66F-D43E-1749-A212-4ECD819803F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="design" sheetId="2" r:id="rId2"/>
+    <sheet name="main" sheetId="3" r:id="rId3"/>
+    <sheet name="output" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="112">
   <si>
     <t>T2</t>
   </si>
@@ -120,13 +123,265 @@
   </si>
   <si>
     <t>TMA112</t>
+  </si>
+  <si>
+    <t>## Input sheet</t>
+  </si>
+  <si>
+    <t>TKB Sheet</t>
+  </si>
+  <si>
+    <t>## Main working sheet</t>
+  </si>
+  <si>
+    <t>1.3Ca1</t>
+  </si>
+  <si>
+    <t>1.2Ca1</t>
+  </si>
+  <si>
+    <t>1.5Ca1</t>
+  </si>
+  <si>
+    <t>1.6Ca1</t>
+  </si>
+  <si>
+    <t>1.2Ca2</t>
+  </si>
+  <si>
+    <t>1.3Ca2</t>
+  </si>
+  <si>
+    <t>1.5Ca2</t>
+  </si>
+  <si>
+    <t>1.6Ca3</t>
+  </si>
+  <si>
+    <t>1.6Ca2</t>
+  </si>
+  <si>
+    <t>1.2Ca3</t>
+  </si>
+  <si>
+    <t>1.3Ca4</t>
+  </si>
+  <si>
+    <t>1.3Ca3</t>
+  </si>
+  <si>
+    <t>1.5Ca3</t>
+  </si>
+  <si>
+    <t>1.2Ca4</t>
+  </si>
+  <si>
+    <t>1.5Ca4</t>
+  </si>
+  <si>
+    <t>1.6Ca4</t>
+  </si>
+  <si>
+    <t>2.3Ca1</t>
+  </si>
+  <si>
+    <t>2.5Ca1</t>
+  </si>
+  <si>
+    <t>2.6Ca1</t>
+  </si>
+  <si>
+    <t>2.2Ca2</t>
+  </si>
+  <si>
+    <t>2.2Ca1</t>
+  </si>
+  <si>
+    <t>2.3Ca2</t>
+  </si>
+  <si>
+    <t>2.5Ca2</t>
+  </si>
+  <si>
+    <t>2.6Ca2</t>
+  </si>
+  <si>
+    <t>2.2Ca3</t>
+  </si>
+  <si>
+    <t>2.3Ca3</t>
+  </si>
+  <si>
+    <t>2.5Ca3</t>
+  </si>
+  <si>
+    <t>2.6Ca3</t>
+  </si>
+  <si>
+    <t>2.2Ca4</t>
+  </si>
+  <si>
+    <t>2.3Ca4</t>
+  </si>
+  <si>
+    <t>2.5Ca4</t>
+  </si>
+  <si>
+    <t>2.6Ca4</t>
+  </si>
+  <si>
+    <t>Subject1</t>
+  </si>
+  <si>
+    <t>Subject2</t>
+  </si>
+  <si>
+    <t>Subject3</t>
+  </si>
+  <si>
+    <t>Subject4</t>
+  </si>
+  <si>
+    <t>Subject5</t>
+  </si>
+  <si>
+    <t>Subject6</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>sep</t>
+  </si>
+  <si>
+    <t>2Ca1.1</t>
+  </si>
+  <si>
+    <t>3Ca1.1</t>
+  </si>
+  <si>
+    <t>5Ca1.1</t>
+  </si>
+  <si>
+    <t>6Ca1.1</t>
+  </si>
+  <si>
+    <t>2Ca2.1</t>
+  </si>
+  <si>
+    <t>3Ca2.1</t>
+  </si>
+  <si>
+    <t>5Ca2.1</t>
+  </si>
+  <si>
+    <t>6Ca2.1</t>
+  </si>
+  <si>
+    <t>2Ca3.1</t>
+  </si>
+  <si>
+    <t>3Ca3.1</t>
+  </si>
+  <si>
+    <t>5Ca3.1</t>
+  </si>
+  <si>
+    <t>6Ca3.1</t>
+  </si>
+  <si>
+    <t>2Ca4.1</t>
+  </si>
+  <si>
+    <t>3Ca4.1</t>
+  </si>
+  <si>
+    <t>5Ca4.1</t>
+  </si>
+  <si>
+    <t>6Ca4.1</t>
+  </si>
+  <si>
+    <t>2Ca1.2</t>
+  </si>
+  <si>
+    <t>3Ca1.2</t>
+  </si>
+  <si>
+    <t>5Ca1.2</t>
+  </si>
+  <si>
+    <t>6Ca1.2</t>
+  </si>
+  <si>
+    <t>2Ca2.2</t>
+  </si>
+  <si>
+    <t>3Ca2.2</t>
+  </si>
+  <si>
+    <t>5Ca2.2</t>
+  </si>
+  <si>
+    <t>6Ca2.2</t>
+  </si>
+  <si>
+    <t>2Ca3.2</t>
+  </si>
+  <si>
+    <t>3Ca3.2</t>
+  </si>
+  <si>
+    <t>5Ca3.2</t>
+  </si>
+  <si>
+    <t>6Ca3.2</t>
+  </si>
+  <si>
+    <t>2Ca4.2</t>
+  </si>
+  <si>
+    <t>3Ca4.2</t>
+  </si>
+  <si>
+    <t>5Ca4.2</t>
+  </si>
+  <si>
+    <t>6Ca4.2</t>
+  </si>
+  <si>
+    <t>Ca1.1</t>
+  </si>
+  <si>
+    <t>Ca2.1</t>
+  </si>
+  <si>
+    <t>Ca3.1</t>
+  </si>
+  <si>
+    <t>Ca4.1</t>
+  </si>
+  <si>
+    <t>Ca1.2</t>
+  </si>
+  <si>
+    <t>Ca2.2</t>
+  </si>
+  <si>
+    <t>Ca3.2</t>
+  </si>
+  <si>
+    <t>Ca4.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,6 +393,19 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -255,13 +523,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,7 +846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1607F20B-1619-1F42-A6EE-036B02C3C906}">
   <dimension ref="A2:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -609,19 +877,19 @@
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3">
         <v>3</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3">
         <v>4</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>5</v>
       </c>
     </row>
@@ -629,19 +897,19 @@
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4">
         <v>6</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4">
         <v>7</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>8</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4">
         <v>9</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>10</v>
       </c>
     </row>
@@ -649,58 +917,58 @@
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5">
         <v>11</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5">
         <v>12</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5">
         <v>13</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5">
         <v>14</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>16</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>17</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>18</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>19</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -719,7 +987,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -805,6 +1073,772 @@
       </c>
       <c r="F25">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEECC2EE-7759-BC48-904C-FF80B11CEEC8}">
+  <dimension ref="A1:I45"/>
+  <sheetViews>
+    <sheetView zoomScale="144" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f>SUM(C6:H6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7:I45" si="0">SUM(C7:H7)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>45</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>49</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>53</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>54</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>56</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>57</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>58</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>59</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>60</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>61</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>62</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1BADEA2-5FAF-7E43-A92F-FC2D460BD5DE}">
+  <dimension ref="A1:A41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE59BFB-8F85-DB40-805B-C4FA87A6430F}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="10">
+        <v>2</v>
+      </c>
+      <c r="C1" s="10">
+        <v>3</v>
+      </c>
+      <c r="D1" s="10">
+        <v>4</v>
+      </c>
+      <c r="E1" s="10">
+        <v>5</v>
+      </c>
+      <c r="F1" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>